<commit_message>
Duplicate number issue fixed
</commit_message>
<xml_diff>
--- a/migration/backend/storage/sheets/common/7b843c49-bfe7-11f0-ad7f-40c2baaf5526/2025-Odd-Sem-Sem-3.xlsx
+++ b/migration/backend/storage/sheets/common/7b843c49-bfe7-11f0-ad7f-40c2baaf5526/2025-Odd-Sem-Sem-3.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -467,6 +467,9 @@
         <v>duplicate number</v>
       </c>
       <c r="V1" t="str">
+        <v>__EMPTY</v>
+      </c>
+      <c r="W1" t="str">
         <v>2 Marks</v>
       </c>
     </row>
@@ -517,22 +520,22 @@
         <v/>
       </c>
       <c r="P2" t="str">
-        <v>2403617615921011</v>
+        <v>2403617615921016</v>
       </c>
       <c r="Q2" t="str">
-        <v>240361761592011</v>
+        <v>240361761592016</v>
       </c>
       <c r="R2" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="T2" t="str">
         <v>Present</v>
       </c>
       <c r="U2">
-        <v>1001</v>
+        <v>555001</v>
       </c>
       <c r="V2" t="str">
         <v/>
@@ -585,22 +588,22 @@
         <v/>
       </c>
       <c r="P3" t="str">
-        <v>2403617615921012</v>
+        <v>2403617615921017</v>
       </c>
       <c r="Q3" t="str">
-        <v>240361761592012</v>
+        <v>240361761592017</v>
       </c>
       <c r="R3" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S3">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="T3" t="str">
         <v>Present</v>
       </c>
       <c r="U3">
-        <v>1002</v>
+        <v>555002</v>
       </c>
       <c r="V3" t="str">
         <v/>
@@ -653,22 +656,22 @@
         <v/>
       </c>
       <c r="P4" t="str">
-        <v>2403617615921013</v>
+        <v>2403617615921018</v>
       </c>
       <c r="Q4" t="str">
-        <v>240361761592013</v>
+        <v>240361761592018</v>
       </c>
       <c r="R4" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S4">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="T4" t="str">
         <v>Present</v>
       </c>
       <c r="U4">
-        <v>1003</v>
+        <v>555003</v>
       </c>
       <c r="V4" t="str">
         <v/>
@@ -721,22 +724,22 @@
         <v/>
       </c>
       <c r="P5" t="str">
-        <v>2403617615921014</v>
+        <v>2403617615921019</v>
       </c>
       <c r="Q5" t="str">
-        <v>240361761592014</v>
+        <v>240361761592019</v>
       </c>
       <c r="R5" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S5">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="T5" t="str">
         <v>Present</v>
       </c>
       <c r="U5">
-        <v>1004</v>
+        <v>555004</v>
       </c>
       <c r="V5" t="str">
         <v/>
@@ -789,22 +792,22 @@
         <v/>
       </c>
       <c r="P6" t="str">
-        <v>2403617615921015</v>
+        <v>2403617615921020</v>
       </c>
       <c r="Q6" t="str">
-        <v>240361761592015</v>
+        <v>240361761592020</v>
       </c>
       <c r="R6" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S6">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="T6" t="str">
         <v>Present</v>
       </c>
       <c r="U6">
-        <v>1005</v>
+        <v>555005</v>
       </c>
       <c r="V6" t="str">
         <v/>
@@ -872,7 +875,7 @@
         <v>Present</v>
       </c>
       <c r="U7">
-        <v>1006</v>
+        <v>555006</v>
       </c>
       <c r="V7" t="str">
         <v/>
@@ -940,7 +943,7 @@
         <v>Present</v>
       </c>
       <c r="U8">
-        <v>1007</v>
+        <v>555007</v>
       </c>
       <c r="V8" t="str">
         <v/>
@@ -1008,7 +1011,7 @@
         <v>Present</v>
       </c>
       <c r="U9">
-        <v>1008</v>
+        <v>555008</v>
       </c>
       <c r="V9" t="str">
         <v/>
@@ -1076,7 +1079,7 @@
         <v>Present</v>
       </c>
       <c r="U10">
-        <v>1009</v>
+        <v>555009</v>
       </c>
       <c r="V10" t="str">
         <v/>
@@ -1144,7 +1147,7 @@
         <v>Present</v>
       </c>
       <c r="U11">
-        <v>1010</v>
+        <v>555010</v>
       </c>
       <c r="V11" t="str">
         <v/>
@@ -1197,22 +1200,22 @@
         <v/>
       </c>
       <c r="P12" t="str">
-        <v>2403617615921016</v>
+        <v>2403617615921011</v>
       </c>
       <c r="Q12" t="str">
-        <v>240361761592016</v>
+        <v>240361761592011</v>
       </c>
       <c r="R12" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S12">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="T12" t="str">
         <v>Present</v>
       </c>
       <c r="U12">
-        <v>1011</v>
+        <v>555011</v>
       </c>
       <c r="V12" t="str">
         <v/>
@@ -1265,22 +1268,22 @@
         <v/>
       </c>
       <c r="P13" t="str">
-        <v>2403617615921017</v>
+        <v>2403617615921012</v>
       </c>
       <c r="Q13" t="str">
-        <v>240361761592017</v>
+        <v>240361761592012</v>
       </c>
       <c r="R13" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S13">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="T13" t="str">
         <v>Present</v>
       </c>
       <c r="U13">
-        <v>1012</v>
+        <v>555012</v>
       </c>
       <c r="V13" t="str">
         <v/>
@@ -1333,22 +1336,22 @@
         <v/>
       </c>
       <c r="P14" t="str">
-        <v>2403617615921018</v>
+        <v>2403617615921013</v>
       </c>
       <c r="Q14" t="str">
-        <v>240361761592018</v>
+        <v>240361761592013</v>
       </c>
       <c r="R14" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S14">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="T14" t="str">
         <v>Present</v>
       </c>
       <c r="U14">
-        <v>1013</v>
+        <v>555013</v>
       </c>
       <c r="V14" t="str">
         <v/>
@@ -1401,22 +1404,22 @@
         <v/>
       </c>
       <c r="P15" t="str">
-        <v>2403617615921019</v>
+        <v>2403617615921014</v>
       </c>
       <c r="Q15" t="str">
-        <v>240361761592019</v>
+        <v>240361761592014</v>
       </c>
       <c r="R15" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S15">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="T15" t="str">
         <v>Present</v>
       </c>
       <c r="U15">
-        <v>1014</v>
+        <v>555014</v>
       </c>
       <c r="V15" t="str">
         <v/>
@@ -1469,22 +1472,22 @@
         <v/>
       </c>
       <c r="P16" t="str">
-        <v>2403617615921020</v>
+        <v>2403617615921015</v>
       </c>
       <c r="Q16" t="str">
-        <v>240361761592020</v>
+        <v>240361761592015</v>
       </c>
       <c r="R16" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S16">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="T16" t="str">
         <v>Present</v>
       </c>
       <c r="U16">
-        <v>1015</v>
+        <v>555015</v>
       </c>
       <c r="V16" t="str">
         <v/>
@@ -1537,10 +1540,10 @@
         <v/>
       </c>
       <c r="P17" t="str">
-        <v>2403617615921021</v>
+        <v>2403617615921006</v>
       </c>
       <c r="Q17" t="str">
-        <v>240361761592021</v>
+        <v>240361761592006</v>
       </c>
       <c r="R17" t="str">
         <v>322CIT05</v>
@@ -1552,7 +1555,7 @@
         <v>Present</v>
       </c>
       <c r="U17">
-        <v>1016</v>
+        <v>555016</v>
       </c>
       <c r="V17" t="str">
         <v/>
@@ -1605,10 +1608,10 @@
         <v/>
       </c>
       <c r="P18" t="str">
-        <v>2403617615921022</v>
+        <v>2403617615921007</v>
       </c>
       <c r="Q18" t="str">
-        <v>240361761592022</v>
+        <v>240361761592007</v>
       </c>
       <c r="R18" t="str">
         <v>322CIT05</v>
@@ -1620,7 +1623,7 @@
         <v>Present</v>
       </c>
       <c r="U18">
-        <v>1017</v>
+        <v>555017</v>
       </c>
       <c r="V18" t="str">
         <v/>
@@ -1673,10 +1676,10 @@
         <v/>
       </c>
       <c r="P19" t="str">
-        <v>2403617615921023</v>
+        <v>2403617615921008</v>
       </c>
       <c r="Q19" t="str">
-        <v>240361761592023</v>
+        <v>240361761592008</v>
       </c>
       <c r="R19" t="str">
         <v>322CIT05</v>
@@ -1688,7 +1691,7 @@
         <v>Present</v>
       </c>
       <c r="U19">
-        <v>1018</v>
+        <v>555018</v>
       </c>
       <c r="V19" t="str">
         <v/>
@@ -1741,10 +1744,10 @@
         <v/>
       </c>
       <c r="P20" t="str">
-        <v>2403617615921024</v>
+        <v>2403617615921009</v>
       </c>
       <c r="Q20" t="str">
-        <v>240361761592024</v>
+        <v>240361761592009</v>
       </c>
       <c r="R20" t="str">
         <v>322CIT05</v>
@@ -1756,7 +1759,7 @@
         <v>Present</v>
       </c>
       <c r="U20">
-        <v>1019</v>
+        <v>555019</v>
       </c>
       <c r="V20" t="str">
         <v/>
@@ -1809,22 +1812,22 @@
         <v/>
       </c>
       <c r="P21" t="str">
-        <v>2403617615921025</v>
+        <v>2403617615921010</v>
       </c>
       <c r="Q21" t="str">
-        <v>240361761592025</v>
+        <v>240361761592010</v>
       </c>
       <c r="R21" t="str">
         <v>322CIT05</v>
       </c>
       <c r="S21">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="T21" t="str">
         <v>Present</v>
       </c>
       <c r="U21">
-        <v>1020</v>
+        <v>555020</v>
       </c>
       <c r="V21" t="str">
         <v/>
@@ -1877,10 +1880,10 @@
         <v/>
       </c>
       <c r="P22" t="str">
-        <v>2403617615921006</v>
+        <v>2403617614921006</v>
       </c>
       <c r="Q22" t="str">
-        <v>240361761592006</v>
+        <v>240361761492006</v>
       </c>
       <c r="R22" t="str">
         <v>322CIT05</v>
@@ -1892,9 +1895,9 @@
         <v>Present</v>
       </c>
       <c r="U22">
-        <v>1021</v>
-      </c>
-      <c r="V22" t="str">
+        <v>555021</v>
+      </c>
+      <c r="W22" t="str">
         <v/>
       </c>
     </row>
@@ -1945,10 +1948,10 @@
         <v/>
       </c>
       <c r="P23" t="str">
-        <v>2403617615921007</v>
+        <v>2403617614921007</v>
       </c>
       <c r="Q23" t="str">
-        <v>240361761592007</v>
+        <v>240361761492007</v>
       </c>
       <c r="R23" t="str">
         <v>322CIT05</v>
@@ -1960,9 +1963,9 @@
         <v>Present</v>
       </c>
       <c r="U23">
-        <v>1022</v>
-      </c>
-      <c r="V23" t="str">
+        <v>555022</v>
+      </c>
+      <c r="W23" t="str">
         <v/>
       </c>
     </row>
@@ -2013,10 +2016,10 @@
         <v/>
       </c>
       <c r="P24" t="str">
-        <v>2403617615921008</v>
+        <v>2403617614921008</v>
       </c>
       <c r="Q24" t="str">
-        <v>240361761592008</v>
+        <v>240361761492008</v>
       </c>
       <c r="R24" t="str">
         <v>322CIT05</v>
@@ -2028,9 +2031,9 @@
         <v>Present</v>
       </c>
       <c r="U24">
-        <v>1023</v>
-      </c>
-      <c r="V24" t="str">
+        <v>555023</v>
+      </c>
+      <c r="W24" t="str">
         <v/>
       </c>
     </row>
@@ -2081,10 +2084,10 @@
         <v/>
       </c>
       <c r="P25" t="str">
-        <v>2403617615921009</v>
+        <v>2403617614921009</v>
       </c>
       <c r="Q25" t="str">
-        <v>240361761592009</v>
+        <v>240361761492009</v>
       </c>
       <c r="R25" t="str">
         <v>322CIT05</v>
@@ -2096,9 +2099,9 @@
         <v>Present</v>
       </c>
       <c r="U25">
-        <v>1024</v>
-      </c>
-      <c r="V25" t="str">
+        <v>555024</v>
+      </c>
+      <c r="W25" t="str">
         <v/>
       </c>
     </row>
@@ -2149,10 +2152,10 @@
         <v/>
       </c>
       <c r="P26" t="str">
-        <v>2403617615921010</v>
+        <v>2403617614921010</v>
       </c>
       <c r="Q26" t="str">
-        <v>240361761592010</v>
+        <v>240361761492010</v>
       </c>
       <c r="R26" t="str">
         <v>322CIT05</v>
@@ -2164,15 +2167,1647 @@
         <v>Present</v>
       </c>
       <c r="U26">
-        <v>1025</v>
-      </c>
-      <c r="V26" t="str">
+        <v>555025</v>
+      </c>
+      <c r="W26" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v/>
+      </c>
+      <c r="B27" t="str">
+        <v/>
+      </c>
+      <c r="C27" t="str">
+        <v/>
+      </c>
+      <c r="D27" t="str">
+        <v/>
+      </c>
+      <c r="E27" t="str">
+        <v/>
+      </c>
+      <c r="F27" t="str">
+        <v/>
+      </c>
+      <c r="G27" t="str">
+        <v/>
+      </c>
+      <c r="H27" t="str">
+        <v/>
+      </c>
+      <c r="I27" t="str">
+        <v/>
+      </c>
+      <c r="J27" t="str">
+        <v/>
+      </c>
+      <c r="K27" t="str">
+        <v/>
+      </c>
+      <c r="L27" t="str">
+        <v/>
+      </c>
+      <c r="M27" t="str">
+        <v/>
+      </c>
+      <c r="N27" t="str">
+        <v/>
+      </c>
+      <c r="O27" t="str">
+        <v/>
+      </c>
+      <c r="P27" t="str">
+        <v>2403617614921011</v>
+      </c>
+      <c r="Q27" t="str">
+        <v>240361761492011</v>
+      </c>
+      <c r="R27" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S27">
+        <v>20</v>
+      </c>
+      <c r="T27" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U27">
+        <v>555026</v>
+      </c>
+      <c r="W27" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v/>
+      </c>
+      <c r="B28" t="str">
+        <v/>
+      </c>
+      <c r="C28" t="str">
+        <v/>
+      </c>
+      <c r="D28" t="str">
+        <v/>
+      </c>
+      <c r="E28" t="str">
+        <v/>
+      </c>
+      <c r="F28" t="str">
+        <v/>
+      </c>
+      <c r="G28" t="str">
+        <v/>
+      </c>
+      <c r="H28" t="str">
+        <v/>
+      </c>
+      <c r="I28" t="str">
+        <v/>
+      </c>
+      <c r="J28" t="str">
+        <v/>
+      </c>
+      <c r="K28" t="str">
+        <v/>
+      </c>
+      <c r="L28" t="str">
+        <v/>
+      </c>
+      <c r="M28" t="str">
+        <v/>
+      </c>
+      <c r="N28" t="str">
+        <v/>
+      </c>
+      <c r="O28" t="str">
+        <v/>
+      </c>
+      <c r="P28" t="str">
+        <v>2403617614921012</v>
+      </c>
+      <c r="Q28" t="str">
+        <v>240361761492012</v>
+      </c>
+      <c r="R28" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S28">
+        <v>21</v>
+      </c>
+      <c r="T28" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U28">
+        <v>555027</v>
+      </c>
+      <c r="W28" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v/>
+      </c>
+      <c r="B29" t="str">
+        <v/>
+      </c>
+      <c r="C29" t="str">
+        <v/>
+      </c>
+      <c r="D29" t="str">
+        <v/>
+      </c>
+      <c r="E29" t="str">
+        <v/>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+      <c r="G29" t="str">
+        <v/>
+      </c>
+      <c r="H29" t="str">
+        <v/>
+      </c>
+      <c r="I29" t="str">
+        <v/>
+      </c>
+      <c r="J29" t="str">
+        <v/>
+      </c>
+      <c r="K29" t="str">
+        <v/>
+      </c>
+      <c r="L29" t="str">
+        <v/>
+      </c>
+      <c r="M29" t="str">
+        <v/>
+      </c>
+      <c r="N29" t="str">
+        <v/>
+      </c>
+      <c r="O29" t="str">
+        <v/>
+      </c>
+      <c r="P29" t="str">
+        <v>2403617614921013</v>
+      </c>
+      <c r="Q29" t="str">
+        <v>240361761492013</v>
+      </c>
+      <c r="R29" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S29">
+        <v>22</v>
+      </c>
+      <c r="T29" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U29">
+        <v>555028</v>
+      </c>
+      <c r="W29" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v/>
+      </c>
+      <c r="B30" t="str">
+        <v/>
+      </c>
+      <c r="C30" t="str">
+        <v/>
+      </c>
+      <c r="D30" t="str">
+        <v/>
+      </c>
+      <c r="E30" t="str">
+        <v/>
+      </c>
+      <c r="F30" t="str">
+        <v/>
+      </c>
+      <c r="G30" t="str">
+        <v/>
+      </c>
+      <c r="H30" t="str">
+        <v/>
+      </c>
+      <c r="I30" t="str">
+        <v/>
+      </c>
+      <c r="J30" t="str">
+        <v/>
+      </c>
+      <c r="K30" t="str">
+        <v/>
+      </c>
+      <c r="L30" t="str">
+        <v/>
+      </c>
+      <c r="M30" t="str">
+        <v/>
+      </c>
+      <c r="N30" t="str">
+        <v/>
+      </c>
+      <c r="O30" t="str">
+        <v/>
+      </c>
+      <c r="P30" t="str">
+        <v>2403617614921014</v>
+      </c>
+      <c r="Q30" t="str">
+        <v>240361761492014</v>
+      </c>
+      <c r="R30" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S30">
+        <v>23</v>
+      </c>
+      <c r="T30" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U30">
+        <v>555029</v>
+      </c>
+      <c r="W30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v/>
+      </c>
+      <c r="B31" t="str">
+        <v/>
+      </c>
+      <c r="C31" t="str">
+        <v/>
+      </c>
+      <c r="D31" t="str">
+        <v/>
+      </c>
+      <c r="E31" t="str">
+        <v/>
+      </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
+      <c r="G31" t="str">
+        <v/>
+      </c>
+      <c r="H31" t="str">
+        <v/>
+      </c>
+      <c r="I31" t="str">
+        <v/>
+      </c>
+      <c r="J31" t="str">
+        <v/>
+      </c>
+      <c r="K31" t="str">
+        <v/>
+      </c>
+      <c r="L31" t="str">
+        <v/>
+      </c>
+      <c r="M31" t="str">
+        <v/>
+      </c>
+      <c r="N31" t="str">
+        <v/>
+      </c>
+      <c r="O31" t="str">
+        <v/>
+      </c>
+      <c r="P31" t="str">
+        <v>2403617614921015</v>
+      </c>
+      <c r="Q31" t="str">
+        <v>240361761492015</v>
+      </c>
+      <c r="R31" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S31">
+        <v>24</v>
+      </c>
+      <c r="T31" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U31">
+        <v>555030</v>
+      </c>
+      <c r="W31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v/>
+      </c>
+      <c r="B32" t="str">
+        <v/>
+      </c>
+      <c r="C32" t="str">
+        <v/>
+      </c>
+      <c r="D32" t="str">
+        <v/>
+      </c>
+      <c r="E32" t="str">
+        <v/>
+      </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
+      <c r="G32" t="str">
+        <v/>
+      </c>
+      <c r="H32" t="str">
+        <v/>
+      </c>
+      <c r="I32" t="str">
+        <v/>
+      </c>
+      <c r="J32" t="str">
+        <v/>
+      </c>
+      <c r="K32" t="str">
+        <v/>
+      </c>
+      <c r="L32" t="str">
+        <v/>
+      </c>
+      <c r="M32" t="str">
+        <v/>
+      </c>
+      <c r="N32" t="str">
+        <v/>
+      </c>
+      <c r="O32" t="str">
+        <v/>
+      </c>
+      <c r="P32" t="str">
+        <v>2403617615921021</v>
+      </c>
+      <c r="Q32" t="str">
+        <v>240361761592021</v>
+      </c>
+      <c r="R32" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S32">
+        <v>30</v>
+      </c>
+      <c r="T32" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U32">
+        <v>555031</v>
+      </c>
+      <c r="V32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v/>
+      </c>
+      <c r="B33" t="str">
+        <v/>
+      </c>
+      <c r="C33" t="str">
+        <v/>
+      </c>
+      <c r="D33" t="str">
+        <v/>
+      </c>
+      <c r="E33" t="str">
+        <v/>
+      </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
+      <c r="G33" t="str">
+        <v/>
+      </c>
+      <c r="H33" t="str">
+        <v/>
+      </c>
+      <c r="I33" t="str">
+        <v/>
+      </c>
+      <c r="J33" t="str">
+        <v/>
+      </c>
+      <c r="K33" t="str">
+        <v/>
+      </c>
+      <c r="L33" t="str">
+        <v/>
+      </c>
+      <c r="M33" t="str">
+        <v/>
+      </c>
+      <c r="N33" t="str">
+        <v/>
+      </c>
+      <c r="O33" t="str">
+        <v/>
+      </c>
+      <c r="P33" t="str">
+        <v>2403617615921022</v>
+      </c>
+      <c r="Q33" t="str">
+        <v>240361761592022</v>
+      </c>
+      <c r="R33" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S33">
+        <v>31</v>
+      </c>
+      <c r="T33" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U33">
+        <v>555032</v>
+      </c>
+      <c r="V33" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v/>
+      </c>
+      <c r="B34" t="str">
+        <v/>
+      </c>
+      <c r="C34" t="str">
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <v/>
+      </c>
+      <c r="E34" t="str">
+        <v/>
+      </c>
+      <c r="F34" t="str">
+        <v/>
+      </c>
+      <c r="G34" t="str">
+        <v/>
+      </c>
+      <c r="H34" t="str">
+        <v/>
+      </c>
+      <c r="I34" t="str">
+        <v/>
+      </c>
+      <c r="J34" t="str">
+        <v/>
+      </c>
+      <c r="K34" t="str">
+        <v/>
+      </c>
+      <c r="L34" t="str">
+        <v/>
+      </c>
+      <c r="M34" t="str">
+        <v/>
+      </c>
+      <c r="N34" t="str">
+        <v/>
+      </c>
+      <c r="O34" t="str">
+        <v/>
+      </c>
+      <c r="P34" t="str">
+        <v>2403617615921023</v>
+      </c>
+      <c r="Q34" t="str">
+        <v>240361761592023</v>
+      </c>
+      <c r="R34" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S34">
+        <v>32</v>
+      </c>
+      <c r="T34" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U34">
+        <v>555033</v>
+      </c>
+      <c r="V34" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v/>
+      </c>
+      <c r="B35" t="str">
+        <v/>
+      </c>
+      <c r="C35" t="str">
+        <v/>
+      </c>
+      <c r="D35" t="str">
+        <v/>
+      </c>
+      <c r="E35" t="str">
+        <v/>
+      </c>
+      <c r="F35" t="str">
+        <v/>
+      </c>
+      <c r="G35" t="str">
+        <v/>
+      </c>
+      <c r="H35" t="str">
+        <v/>
+      </c>
+      <c r="I35" t="str">
+        <v/>
+      </c>
+      <c r="J35" t="str">
+        <v/>
+      </c>
+      <c r="K35" t="str">
+        <v/>
+      </c>
+      <c r="L35" t="str">
+        <v/>
+      </c>
+      <c r="M35" t="str">
+        <v/>
+      </c>
+      <c r="N35" t="str">
+        <v/>
+      </c>
+      <c r="O35" t="str">
+        <v/>
+      </c>
+      <c r="P35" t="str">
+        <v>2403617614921016</v>
+      </c>
+      <c r="Q35" t="str">
+        <v>240361761492016</v>
+      </c>
+      <c r="R35" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S35">
+        <v>25</v>
+      </c>
+      <c r="T35" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U35">
+        <v>555034</v>
+      </c>
+      <c r="W35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v/>
+      </c>
+      <c r="B36" t="str">
+        <v/>
+      </c>
+      <c r="C36" t="str">
+        <v/>
+      </c>
+      <c r="D36" t="str">
+        <v/>
+      </c>
+      <c r="E36" t="str">
+        <v/>
+      </c>
+      <c r="F36" t="str">
+        <v/>
+      </c>
+      <c r="G36" t="str">
+        <v/>
+      </c>
+      <c r="H36" t="str">
+        <v/>
+      </c>
+      <c r="I36" t="str">
+        <v/>
+      </c>
+      <c r="J36" t="str">
+        <v/>
+      </c>
+      <c r="K36" t="str">
+        <v/>
+      </c>
+      <c r="L36" t="str">
+        <v/>
+      </c>
+      <c r="M36" t="str">
+        <v/>
+      </c>
+      <c r="N36" t="str">
+        <v/>
+      </c>
+      <c r="O36" t="str">
+        <v/>
+      </c>
+      <c r="P36" t="str">
+        <v>2403617614921017</v>
+      </c>
+      <c r="Q36" t="str">
+        <v>240361761492017</v>
+      </c>
+      <c r="R36" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S36">
+        <v>26</v>
+      </c>
+      <c r="T36" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U36">
+        <v>555035</v>
+      </c>
+      <c r="W36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v/>
+      </c>
+      <c r="B37" t="str">
+        <v/>
+      </c>
+      <c r="C37" t="str">
+        <v/>
+      </c>
+      <c r="D37" t="str">
+        <v/>
+      </c>
+      <c r="E37" t="str">
+        <v/>
+      </c>
+      <c r="F37" t="str">
+        <v/>
+      </c>
+      <c r="G37" t="str">
+        <v/>
+      </c>
+      <c r="H37" t="str">
+        <v/>
+      </c>
+      <c r="I37" t="str">
+        <v/>
+      </c>
+      <c r="J37" t="str">
+        <v/>
+      </c>
+      <c r="K37" t="str">
+        <v/>
+      </c>
+      <c r="L37" t="str">
+        <v/>
+      </c>
+      <c r="M37" t="str">
+        <v/>
+      </c>
+      <c r="N37" t="str">
+        <v/>
+      </c>
+      <c r="O37" t="str">
+        <v/>
+      </c>
+      <c r="P37" t="str">
+        <v>2403617614921018</v>
+      </c>
+      <c r="Q37" t="str">
+        <v>240361761492018</v>
+      </c>
+      <c r="R37" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S37">
+        <v>27</v>
+      </c>
+      <c r="T37" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U37">
+        <v>555036</v>
+      </c>
+      <c r="W37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v/>
+      </c>
+      <c r="B38" t="str">
+        <v/>
+      </c>
+      <c r="C38" t="str">
+        <v/>
+      </c>
+      <c r="D38" t="str">
+        <v/>
+      </c>
+      <c r="E38" t="str">
+        <v/>
+      </c>
+      <c r="F38" t="str">
+        <v/>
+      </c>
+      <c r="G38" t="str">
+        <v/>
+      </c>
+      <c r="H38" t="str">
+        <v/>
+      </c>
+      <c r="I38" t="str">
+        <v/>
+      </c>
+      <c r="J38" t="str">
+        <v/>
+      </c>
+      <c r="K38" t="str">
+        <v/>
+      </c>
+      <c r="L38" t="str">
+        <v/>
+      </c>
+      <c r="M38" t="str">
+        <v/>
+      </c>
+      <c r="N38" t="str">
+        <v/>
+      </c>
+      <c r="O38" t="str">
+        <v/>
+      </c>
+      <c r="P38" t="str">
+        <v>2403617614921019</v>
+      </c>
+      <c r="Q38" t="str">
+        <v>240361761492019</v>
+      </c>
+      <c r="R38" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S38">
+        <v>28</v>
+      </c>
+      <c r="T38" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U38">
+        <v>555037</v>
+      </c>
+      <c r="W38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v/>
+      </c>
+      <c r="B39" t="str">
+        <v/>
+      </c>
+      <c r="C39" t="str">
+        <v/>
+      </c>
+      <c r="D39" t="str">
+        <v/>
+      </c>
+      <c r="E39" t="str">
+        <v/>
+      </c>
+      <c r="F39" t="str">
+        <v/>
+      </c>
+      <c r="G39" t="str">
+        <v/>
+      </c>
+      <c r="H39" t="str">
+        <v/>
+      </c>
+      <c r="I39" t="str">
+        <v/>
+      </c>
+      <c r="J39" t="str">
+        <v/>
+      </c>
+      <c r="K39" t="str">
+        <v/>
+      </c>
+      <c r="L39" t="str">
+        <v/>
+      </c>
+      <c r="M39" t="str">
+        <v/>
+      </c>
+      <c r="N39" t="str">
+        <v/>
+      </c>
+      <c r="O39" t="str">
+        <v/>
+      </c>
+      <c r="P39" t="str">
+        <v>2403617614921020</v>
+      </c>
+      <c r="Q39" t="str">
+        <v>240361761492020</v>
+      </c>
+      <c r="R39" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S39">
+        <v>29</v>
+      </c>
+      <c r="T39" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U39">
+        <v>555038</v>
+      </c>
+      <c r="W39" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v/>
+      </c>
+      <c r="B40" t="str">
+        <v/>
+      </c>
+      <c r="C40" t="str">
+        <v/>
+      </c>
+      <c r="D40" t="str">
+        <v/>
+      </c>
+      <c r="E40" t="str">
+        <v/>
+      </c>
+      <c r="F40" t="str">
+        <v/>
+      </c>
+      <c r="G40" t="str">
+        <v/>
+      </c>
+      <c r="H40" t="str">
+        <v/>
+      </c>
+      <c r="I40" t="str">
+        <v/>
+      </c>
+      <c r="J40" t="str">
+        <v/>
+      </c>
+      <c r="K40" t="str">
+        <v/>
+      </c>
+      <c r="L40" t="str">
+        <v/>
+      </c>
+      <c r="M40" t="str">
+        <v/>
+      </c>
+      <c r="N40" t="str">
+        <v/>
+      </c>
+      <c r="O40" t="str">
+        <v/>
+      </c>
+      <c r="P40" t="str">
+        <v>2403617614921021</v>
+      </c>
+      <c r="Q40" t="str">
+        <v>240361761492021</v>
+      </c>
+      <c r="R40" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S40">
+        <v>30</v>
+      </c>
+      <c r="T40" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U40">
+        <v>555039</v>
+      </c>
+      <c r="W40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v/>
+      </c>
+      <c r="B41" t="str">
+        <v/>
+      </c>
+      <c r="C41" t="str">
+        <v/>
+      </c>
+      <c r="D41" t="str">
+        <v/>
+      </c>
+      <c r="E41" t="str">
+        <v/>
+      </c>
+      <c r="F41" t="str">
+        <v/>
+      </c>
+      <c r="G41" t="str">
+        <v/>
+      </c>
+      <c r="H41" t="str">
+        <v/>
+      </c>
+      <c r="I41" t="str">
+        <v/>
+      </c>
+      <c r="J41" t="str">
+        <v/>
+      </c>
+      <c r="K41" t="str">
+        <v/>
+      </c>
+      <c r="L41" t="str">
+        <v/>
+      </c>
+      <c r="M41" t="str">
+        <v/>
+      </c>
+      <c r="N41" t="str">
+        <v/>
+      </c>
+      <c r="O41" t="str">
+        <v/>
+      </c>
+      <c r="P41" t="str">
+        <v>2403617614921022</v>
+      </c>
+      <c r="Q41" t="str">
+        <v>240361761492022</v>
+      </c>
+      <c r="R41" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S41">
+        <v>31</v>
+      </c>
+      <c r="T41" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U41">
+        <v>555040</v>
+      </c>
+      <c r="W41" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v/>
+      </c>
+      <c r="B42" t="str">
+        <v/>
+      </c>
+      <c r="C42" t="str">
+        <v/>
+      </c>
+      <c r="D42" t="str">
+        <v/>
+      </c>
+      <c r="E42" t="str">
+        <v/>
+      </c>
+      <c r="F42" t="str">
+        <v/>
+      </c>
+      <c r="G42" t="str">
+        <v/>
+      </c>
+      <c r="H42" t="str">
+        <v/>
+      </c>
+      <c r="I42" t="str">
+        <v/>
+      </c>
+      <c r="J42" t="str">
+        <v/>
+      </c>
+      <c r="K42" t="str">
+        <v/>
+      </c>
+      <c r="L42" t="str">
+        <v/>
+      </c>
+      <c r="M42" t="str">
+        <v/>
+      </c>
+      <c r="N42" t="str">
+        <v/>
+      </c>
+      <c r="O42" t="str">
+        <v/>
+      </c>
+      <c r="P42" t="str">
+        <v>2403617614921023</v>
+      </c>
+      <c r="Q42" t="str">
+        <v>240361761492023</v>
+      </c>
+      <c r="R42" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S42">
+        <v>32</v>
+      </c>
+      <c r="T42" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U42">
+        <v>555041</v>
+      </c>
+      <c r="W42" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v/>
+      </c>
+      <c r="B43" t="str">
+        <v/>
+      </c>
+      <c r="C43" t="str">
+        <v/>
+      </c>
+      <c r="D43" t="str">
+        <v/>
+      </c>
+      <c r="E43" t="str">
+        <v/>
+      </c>
+      <c r="F43" t="str">
+        <v/>
+      </c>
+      <c r="G43" t="str">
+        <v/>
+      </c>
+      <c r="H43" t="str">
+        <v/>
+      </c>
+      <c r="I43" t="str">
+        <v/>
+      </c>
+      <c r="J43" t="str">
+        <v/>
+      </c>
+      <c r="K43" t="str">
+        <v/>
+      </c>
+      <c r="L43" t="str">
+        <v/>
+      </c>
+      <c r="M43" t="str">
+        <v/>
+      </c>
+      <c r="N43" t="str">
+        <v/>
+      </c>
+      <c r="O43" t="str">
+        <v/>
+      </c>
+      <c r="P43" t="str">
+        <v>2403617614921024</v>
+      </c>
+      <c r="Q43" t="str">
+        <v>240361761492024</v>
+      </c>
+      <c r="R43" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S43">
+        <v>33</v>
+      </c>
+      <c r="T43" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U43">
+        <v>555042</v>
+      </c>
+      <c r="W43" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v/>
+      </c>
+      <c r="B44" t="str">
+        <v/>
+      </c>
+      <c r="C44" t="str">
+        <v/>
+      </c>
+      <c r="D44" t="str">
+        <v/>
+      </c>
+      <c r="E44" t="str">
+        <v/>
+      </c>
+      <c r="F44" t="str">
+        <v/>
+      </c>
+      <c r="G44" t="str">
+        <v/>
+      </c>
+      <c r="H44" t="str">
+        <v/>
+      </c>
+      <c r="I44" t="str">
+        <v/>
+      </c>
+      <c r="J44" t="str">
+        <v/>
+      </c>
+      <c r="K44" t="str">
+        <v/>
+      </c>
+      <c r="L44" t="str">
+        <v/>
+      </c>
+      <c r="M44" t="str">
+        <v/>
+      </c>
+      <c r="N44" t="str">
+        <v/>
+      </c>
+      <c r="O44" t="str">
+        <v/>
+      </c>
+      <c r="P44" t="str">
+        <v>2403617614921025</v>
+      </c>
+      <c r="Q44" t="str">
+        <v>240361761492025</v>
+      </c>
+      <c r="R44" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S44">
+        <v>40</v>
+      </c>
+      <c r="T44" t="str">
+        <v>Present</v>
+      </c>
+      <c r="U44">
+        <v>555043</v>
+      </c>
+      <c r="W44" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v/>
+      </c>
+      <c r="B45" t="str">
+        <v/>
+      </c>
+      <c r="C45" t="str">
+        <v/>
+      </c>
+      <c r="D45" t="str">
+        <v/>
+      </c>
+      <c r="E45" t="str">
+        <v/>
+      </c>
+      <c r="F45" t="str">
+        <v/>
+      </c>
+      <c r="G45" t="str">
+        <v/>
+      </c>
+      <c r="H45" t="str">
+        <v/>
+      </c>
+      <c r="I45" t="str">
+        <v/>
+      </c>
+      <c r="J45" t="str">
+        <v/>
+      </c>
+      <c r="K45" t="str">
+        <v/>
+      </c>
+      <c r="L45" t="str">
+        <v/>
+      </c>
+      <c r="M45" t="str">
+        <v/>
+      </c>
+      <c r="N45" t="str">
+        <v/>
+      </c>
+      <c r="O45" t="str">
+        <v/>
+      </c>
+      <c r="P45" t="str">
+        <v>2403617614921002</v>
+      </c>
+      <c r="Q45" t="str">
+        <v>240361761492002</v>
+      </c>
+      <c r="R45" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S45">
+        <v>26</v>
+      </c>
+      <c r="T45" t="str">
+        <v>Absent</v>
+      </c>
+      <c r="U45" t="str">
+        <v/>
+      </c>
+      <c r="W45" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v/>
+      </c>
+      <c r="B46" t="str">
+        <v/>
+      </c>
+      <c r="C46" t="str">
+        <v/>
+      </c>
+      <c r="D46" t="str">
+        <v/>
+      </c>
+      <c r="E46" t="str">
+        <v/>
+      </c>
+      <c r="F46" t="str">
+        <v/>
+      </c>
+      <c r="G46" t="str">
+        <v/>
+      </c>
+      <c r="H46" t="str">
+        <v/>
+      </c>
+      <c r="I46" t="str">
+        <v/>
+      </c>
+      <c r="J46" t="str">
+        <v/>
+      </c>
+      <c r="K46" t="str">
+        <v/>
+      </c>
+      <c r="L46" t="str">
+        <v/>
+      </c>
+      <c r="M46" t="str">
+        <v/>
+      </c>
+      <c r="N46" t="str">
+        <v/>
+      </c>
+      <c r="O46" t="str">
+        <v/>
+      </c>
+      <c r="P46" t="str">
+        <v>2403617614921003</v>
+      </c>
+      <c r="Q46" t="str">
+        <v>240361761492003</v>
+      </c>
+      <c r="R46" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S46">
+        <v>27</v>
+      </c>
+      <c r="T46" t="str">
+        <v>Absent</v>
+      </c>
+      <c r="U46" t="str">
+        <v/>
+      </c>
+      <c r="W46" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v/>
+      </c>
+      <c r="B47" t="str">
+        <v/>
+      </c>
+      <c r="C47" t="str">
+        <v/>
+      </c>
+      <c r="D47" t="str">
+        <v/>
+      </c>
+      <c r="E47" t="str">
+        <v/>
+      </c>
+      <c r="F47" t="str">
+        <v/>
+      </c>
+      <c r="G47" t="str">
+        <v/>
+      </c>
+      <c r="H47" t="str">
+        <v/>
+      </c>
+      <c r="I47" t="str">
+        <v/>
+      </c>
+      <c r="J47" t="str">
+        <v/>
+      </c>
+      <c r="K47" t="str">
+        <v/>
+      </c>
+      <c r="L47" t="str">
+        <v/>
+      </c>
+      <c r="M47" t="str">
+        <v/>
+      </c>
+      <c r="N47" t="str">
+        <v/>
+      </c>
+      <c r="O47" t="str">
+        <v/>
+      </c>
+      <c r="P47" t="str">
+        <v>2403617614921004</v>
+      </c>
+      <c r="Q47" t="str">
+        <v>240361761492004</v>
+      </c>
+      <c r="R47" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S47">
+        <v>28</v>
+      </c>
+      <c r="T47" t="str">
+        <v>Absent</v>
+      </c>
+      <c r="U47" t="str">
+        <v/>
+      </c>
+      <c r="W47" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v/>
+      </c>
+      <c r="B48" t="str">
+        <v/>
+      </c>
+      <c r="C48" t="str">
+        <v/>
+      </c>
+      <c r="D48" t="str">
+        <v/>
+      </c>
+      <c r="E48" t="str">
+        <v/>
+      </c>
+      <c r="F48" t="str">
+        <v/>
+      </c>
+      <c r="G48" t="str">
+        <v/>
+      </c>
+      <c r="H48" t="str">
+        <v/>
+      </c>
+      <c r="I48" t="str">
+        <v/>
+      </c>
+      <c r="J48" t="str">
+        <v/>
+      </c>
+      <c r="K48" t="str">
+        <v/>
+      </c>
+      <c r="L48" t="str">
+        <v/>
+      </c>
+      <c r="M48" t="str">
+        <v/>
+      </c>
+      <c r="N48" t="str">
+        <v/>
+      </c>
+      <c r="O48" t="str">
+        <v/>
+      </c>
+      <c r="P48" t="str">
+        <v>2403617614921005</v>
+      </c>
+      <c r="Q48" t="str">
+        <v>240361761492005</v>
+      </c>
+      <c r="R48" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S48">
+        <v>29</v>
+      </c>
+      <c r="T48" t="str">
+        <v>Absent</v>
+      </c>
+      <c r="U48" t="str">
+        <v/>
+      </c>
+      <c r="W48" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v/>
+      </c>
+      <c r="B49" t="str">
+        <v/>
+      </c>
+      <c r="C49" t="str">
+        <v/>
+      </c>
+      <c r="D49" t="str">
+        <v/>
+      </c>
+      <c r="E49" t="str">
+        <v/>
+      </c>
+      <c r="F49" t="str">
+        <v/>
+      </c>
+      <c r="G49" t="str">
+        <v/>
+      </c>
+      <c r="H49" t="str">
+        <v/>
+      </c>
+      <c r="I49" t="str">
+        <v/>
+      </c>
+      <c r="J49" t="str">
+        <v/>
+      </c>
+      <c r="K49" t="str">
+        <v/>
+      </c>
+      <c r="L49" t="str">
+        <v/>
+      </c>
+      <c r="M49" t="str">
+        <v/>
+      </c>
+      <c r="N49" t="str">
+        <v/>
+      </c>
+      <c r="O49" t="str">
+        <v/>
+      </c>
+      <c r="P49" t="str">
+        <v>2403617615921024</v>
+      </c>
+      <c r="Q49" t="str">
+        <v>240361761592024</v>
+      </c>
+      <c r="R49" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S49">
+        <v>33</v>
+      </c>
+      <c r="T49" t="str">
+        <v>Absent</v>
+      </c>
+      <c r="U49" t="str">
+        <v/>
+      </c>
+      <c r="V49" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v/>
+      </c>
+      <c r="B50" t="str">
+        <v/>
+      </c>
+      <c r="C50" t="str">
+        <v/>
+      </c>
+      <c r="D50" t="str">
+        <v/>
+      </c>
+      <c r="E50" t="str">
+        <v/>
+      </c>
+      <c r="F50" t="str">
+        <v/>
+      </c>
+      <c r="G50" t="str">
+        <v/>
+      </c>
+      <c r="H50" t="str">
+        <v/>
+      </c>
+      <c r="I50" t="str">
+        <v/>
+      </c>
+      <c r="J50" t="str">
+        <v/>
+      </c>
+      <c r="K50" t="str">
+        <v/>
+      </c>
+      <c r="L50" t="str">
+        <v/>
+      </c>
+      <c r="M50" t="str">
+        <v/>
+      </c>
+      <c r="N50" t="str">
+        <v/>
+      </c>
+      <c r="O50" t="str">
+        <v/>
+      </c>
+      <c r="P50" t="str">
+        <v>2403617615921025</v>
+      </c>
+      <c r="Q50" t="str">
+        <v>240361761592025</v>
+      </c>
+      <c r="R50" t="str">
+        <v>322CIT05</v>
+      </c>
+      <c r="S50">
+        <v>40</v>
+      </c>
+      <c r="T50" t="str">
+        <v>Absent</v>
+      </c>
+      <c r="U50" t="str">
+        <v/>
+      </c>
+      <c r="V50" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:V26"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:W50"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Auto Download Option Added
</commit_message>
<xml_diff>
--- a/migration/backend/storage/sheets/common/7b843c49-bfe7-11f0-ad7f-40c2baaf5526/2025-Odd-Sem-Sem-3.xlsx
+++ b/migration/backend/storage/sheets/common/7b843c49-bfe7-11f0-ad7f-40c2baaf5526/2025-Odd-Sem-Sem-3.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W50"/>
+  <dimension ref="A1:X50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -470,6 +470,9 @@
         <v>__EMPTY</v>
       </c>
       <c r="W1" t="str">
+        <v>Total</v>
+      </c>
+      <c r="X1" t="str">
         <v>2 Marks</v>
       </c>
     </row>
@@ -540,6 +543,9 @@
       <c r="V2" t="str">
         <v/>
       </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -608,6 +614,9 @@
       <c r="V3" t="str">
         <v/>
       </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -676,6 +685,9 @@
       <c r="V4" t="str">
         <v/>
       </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -744,6 +756,9 @@
       <c r="V5" t="str">
         <v/>
       </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -812,6 +827,9 @@
       <c r="V6" t="str">
         <v/>
       </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -880,6 +898,9 @@
       <c r="V7" t="str">
         <v/>
       </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -948,6 +969,9 @@
       <c r="V8" t="str">
         <v/>
       </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -1016,6 +1040,9 @@
       <c r="V9" t="str">
         <v/>
       </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -1084,6 +1111,9 @@
       <c r="V10" t="str">
         <v/>
       </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -1152,6 +1182,9 @@
       <c r="V11" t="str">
         <v/>
       </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -1220,6 +1253,9 @@
       <c r="V12" t="str">
         <v/>
       </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -1288,6 +1324,9 @@
       <c r="V13" t="str">
         <v/>
       </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -1356,6 +1395,9 @@
       <c r="V14" t="str">
         <v/>
       </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -1424,6 +1466,9 @@
       <c r="V15" t="str">
         <v/>
       </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -1492,6 +1537,9 @@
       <c r="V16" t="str">
         <v/>
       </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -1560,6 +1608,9 @@
       <c r="V17" t="str">
         <v/>
       </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1628,6 +1679,9 @@
       <c r="V18" t="str">
         <v/>
       </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -1696,6 +1750,9 @@
       <c r="V19" t="str">
         <v/>
       </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -1764,6 +1821,9 @@
       <c r="V20" t="str">
         <v/>
       </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -1832,6 +1892,9 @@
       <c r="V21" t="str">
         <v/>
       </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1897,7 +1960,10 @@
       <c r="U22">
         <v>555021</v>
       </c>
-      <c r="W22" t="str">
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22" t="str">
         <v/>
       </c>
     </row>
@@ -1965,7 +2031,10 @@
       <c r="U23">
         <v>555022</v>
       </c>
-      <c r="W23" t="str">
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23" t="str">
         <v/>
       </c>
     </row>
@@ -2033,7 +2102,10 @@
       <c r="U24">
         <v>555023</v>
       </c>
-      <c r="W24" t="str">
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24" t="str">
         <v/>
       </c>
     </row>
@@ -2101,7 +2173,10 @@
       <c r="U25">
         <v>555024</v>
       </c>
-      <c r="W25" t="str">
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25" t="str">
         <v/>
       </c>
     </row>
@@ -2169,7 +2244,10 @@
       <c r="U26">
         <v>555025</v>
       </c>
-      <c r="W26" t="str">
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26" t="str">
         <v/>
       </c>
     </row>
@@ -2237,7 +2315,10 @@
       <c r="U27">
         <v>555026</v>
       </c>
-      <c r="W27" t="str">
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27" t="str">
         <v/>
       </c>
     </row>
@@ -2305,7 +2386,10 @@
       <c r="U28">
         <v>555027</v>
       </c>
-      <c r="W28" t="str">
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28" t="str">
         <v/>
       </c>
     </row>
@@ -2373,7 +2457,10 @@
       <c r="U29">
         <v>555028</v>
       </c>
-      <c r="W29" t="str">
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29" t="str">
         <v/>
       </c>
     </row>
@@ -2441,7 +2528,10 @@
       <c r="U30">
         <v>555029</v>
       </c>
-      <c r="W30" t="str">
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30" t="str">
         <v/>
       </c>
     </row>
@@ -2509,7 +2599,10 @@
       <c r="U31">
         <v>555030</v>
       </c>
-      <c r="W31" t="str">
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31" t="str">
         <v/>
       </c>
     </row>
@@ -2580,6 +2673,9 @@
       <c r="V32" t="str">
         <v/>
       </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -2648,6 +2744,9 @@
       <c r="V33" t="str">
         <v/>
       </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -2716,6 +2815,9 @@
       <c r="V34" t="str">
         <v/>
       </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -2781,7 +2883,10 @@
       <c r="U35">
         <v>555034</v>
       </c>
-      <c r="W35" t="str">
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35" t="str">
         <v/>
       </c>
     </row>
@@ -2849,7 +2954,10 @@
       <c r="U36">
         <v>555035</v>
       </c>
-      <c r="W36" t="str">
+      <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36" t="str">
         <v/>
       </c>
     </row>
@@ -2917,7 +3025,10 @@
       <c r="U37">
         <v>555036</v>
       </c>
-      <c r="W37" t="str">
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="X37" t="str">
         <v/>
       </c>
     </row>
@@ -2985,7 +3096,10 @@
       <c r="U38">
         <v>555037</v>
       </c>
-      <c r="W38" t="str">
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="X38" t="str">
         <v/>
       </c>
     </row>
@@ -3053,7 +3167,10 @@
       <c r="U39">
         <v>555038</v>
       </c>
-      <c r="W39" t="str">
+      <c r="W39">
+        <v>0</v>
+      </c>
+      <c r="X39" t="str">
         <v/>
       </c>
     </row>
@@ -3121,7 +3238,10 @@
       <c r="U40">
         <v>555039</v>
       </c>
-      <c r="W40" t="str">
+      <c r="W40">
+        <v>0</v>
+      </c>
+      <c r="X40" t="str">
         <v/>
       </c>
     </row>
@@ -3189,7 +3309,10 @@
       <c r="U41">
         <v>555040</v>
       </c>
-      <c r="W41" t="str">
+      <c r="W41">
+        <v>0</v>
+      </c>
+      <c r="X41" t="str">
         <v/>
       </c>
     </row>
@@ -3257,7 +3380,10 @@
       <c r="U42">
         <v>555041</v>
       </c>
-      <c r="W42" t="str">
+      <c r="W42">
+        <v>0</v>
+      </c>
+      <c r="X42" t="str">
         <v/>
       </c>
     </row>
@@ -3325,7 +3451,10 @@
       <c r="U43">
         <v>555042</v>
       </c>
-      <c r="W43" t="str">
+      <c r="W43">
+        <v>0</v>
+      </c>
+      <c r="X43" t="str">
         <v/>
       </c>
     </row>
@@ -3393,7 +3522,10 @@
       <c r="U44">
         <v>555043</v>
       </c>
-      <c r="W44" t="str">
+      <c r="W44">
+        <v>0</v>
+      </c>
+      <c r="X44" t="str">
         <v/>
       </c>
     </row>
@@ -3461,7 +3593,10 @@
       <c r="U45" t="str">
         <v/>
       </c>
-      <c r="W45" t="str">
+      <c r="W45">
+        <v>0</v>
+      </c>
+      <c r="X45" t="str">
         <v/>
       </c>
     </row>
@@ -3529,7 +3664,10 @@
       <c r="U46" t="str">
         <v/>
       </c>
-      <c r="W46" t="str">
+      <c r="W46">
+        <v>0</v>
+      </c>
+      <c r="X46" t="str">
         <v/>
       </c>
     </row>
@@ -3597,7 +3735,10 @@
       <c r="U47" t="str">
         <v/>
       </c>
-      <c r="W47" t="str">
+      <c r="W47">
+        <v>0</v>
+      </c>
+      <c r="X47" t="str">
         <v/>
       </c>
     </row>
@@ -3665,7 +3806,10 @@
       <c r="U48" t="str">
         <v/>
       </c>
-      <c r="W48" t="str">
+      <c r="W48">
+        <v>0</v>
+      </c>
+      <c r="X48" t="str">
         <v/>
       </c>
     </row>
@@ -3736,6 +3880,9 @@
       <c r="V49" t="str">
         <v/>
       </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -3804,10 +3951,13 @@
       <c r="V50" t="str">
         <v/>
       </c>
+      <c r="W50">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:W50"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:X50"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>